<commit_message>
worked out some bugs
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/Repeater/AAPL/AAPLBag.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/Repeater/AAPL/AAPLBag.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Neutral</t>
+  </si>
+  <si>
+    <t>Up</t>
   </si>
 </sst>
 </file>
@@ -430,9 +433,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y5"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -825,6 +830,468 @@
       <c r="W5">
         <v>0</v>
       </c>
+      <c r="X5">
+        <v>0.18999999999999773</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>42650.338379629633</v>
+      </c>
+      <c r="B6">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6">
+        <v>50</v>
+      </c>
+      <c r="E6">
+        <v>8137</v>
+      </c>
+      <c r="F6">
+        <v>892</v>
+      </c>
+      <c r="G6">
+        <v>68</v>
+      </c>
+      <c r="H6">
+        <v>30</v>
+      </c>
+      <c r="I6">
+        <v>86</v>
+      </c>
+      <c r="J6">
+        <v>13</v>
+      </c>
+      <c r="K6">
+        <v>5412</v>
+      </c>
+      <c r="L6">
+        <v>149</v>
+      </c>
+      <c r="M6">
+        <v>67</v>
+      </c>
+      <c r="N6">
+        <v>59</v>
+      </c>
+      <c r="O6">
+        <v>9</v>
+      </c>
+      <c r="P6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6">
+        <v>38.48959524716075</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6" s="2">
+        <v>0.1046</v>
+      </c>
+      <c r="T6" s="2">
+        <v>3.4500000000000003E-2</v>
+      </c>
+      <c r="U6">
+        <v>4.82</v>
+      </c>
+      <c r="V6">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0.18999999999999773</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>42650.339618055557</v>
+      </c>
+      <c r="B7">
+        <v>-5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>56</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q7">
+        <v>38.48959524716075</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7" s="2">
+        <v>0.1046</v>
+      </c>
+      <c r="T7" s="2">
+        <v>3.4500000000000003E-2</v>
+      </c>
+      <c r="U7">
+        <v>4.82</v>
+      </c>
+      <c r="V7">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0.18999999999999773</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>42650.348773148151</v>
+      </c>
+      <c r="B8">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8">
+        <v>32</v>
+      </c>
+      <c r="E8">
+        <v>33453</v>
+      </c>
+      <c r="F8">
+        <v>3627</v>
+      </c>
+      <c r="G8">
+        <v>61</v>
+      </c>
+      <c r="H8">
+        <v>37</v>
+      </c>
+      <c r="I8">
+        <v>86</v>
+      </c>
+      <c r="J8">
+        <v>13</v>
+      </c>
+      <c r="K8">
+        <v>17329</v>
+      </c>
+      <c r="L8">
+        <v>514</v>
+      </c>
+      <c r="M8">
+        <v>314</v>
+      </c>
+      <c r="N8">
+        <v>84</v>
+      </c>
+      <c r="O8">
+        <v>13</v>
+      </c>
+      <c r="P8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q8">
+        <v>38.48959524716075</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8" s="2">
+        <v>0.1046</v>
+      </c>
+      <c r="T8" s="2">
+        <v>3.4500000000000003E-2</v>
+      </c>
+      <c r="U8">
+        <v>4.82</v>
+      </c>
+      <c r="V8">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="W8">
+        <v>0</v>
+      </c>
+      <c r="X8">
+        <v>0.18999999999999773</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>42650.359050925923</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <v>2806</v>
+      </c>
+      <c r="F9">
+        <v>315</v>
+      </c>
+      <c r="G9">
+        <v>57</v>
+      </c>
+      <c r="H9">
+        <v>42</v>
+      </c>
+      <c r="I9">
+        <v>50</v>
+      </c>
+      <c r="J9">
+        <v>50</v>
+      </c>
+      <c r="K9">
+        <v>2767</v>
+      </c>
+      <c r="L9">
+        <v>41</v>
+      </c>
+      <c r="M9">
+        <v>30</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>1</v>
+      </c>
+      <c r="P9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9">
+        <v>38.48959524716075</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9" s="2">
+        <v>0.1046</v>
+      </c>
+      <c r="T9" s="2">
+        <v>3.4500000000000003E-2</v>
+      </c>
+      <c r="U9">
+        <v>4.82</v>
+      </c>
+      <c r="V9">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0.18999999999999773</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>42650.36146990741</v>
+      </c>
+      <c r="B10">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>50</v>
+      </c>
+      <c r="E10">
+        <v>8149</v>
+      </c>
+      <c r="F10">
+        <v>893</v>
+      </c>
+      <c r="G10">
+        <v>68</v>
+      </c>
+      <c r="H10">
+        <v>30</v>
+      </c>
+      <c r="I10">
+        <v>86</v>
+      </c>
+      <c r="J10">
+        <v>13</v>
+      </c>
+      <c r="K10">
+        <v>5592</v>
+      </c>
+      <c r="L10">
+        <v>149</v>
+      </c>
+      <c r="M10">
+        <v>67</v>
+      </c>
+      <c r="N10">
+        <v>59</v>
+      </c>
+      <c r="O10">
+        <v>9</v>
+      </c>
+      <c r="P10" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q10">
+        <v>38.48959524716075</v>
+      </c>
+      <c r="R10">
+        <v>0</v>
+      </c>
+      <c r="S10" s="2">
+        <v>0.1046</v>
+      </c>
+      <c r="T10" s="2">
+        <v>3.4500000000000003E-2</v>
+      </c>
+      <c r="U10">
+        <v>4.82</v>
+      </c>
+      <c r="V10">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0.18999999999999773</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>42650.36310185185</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>11</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q11">
+        <v>37.799019424898844</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11" s="2">
+        <v>0.1046</v>
+      </c>
+      <c r="T11" s="2">
+        <v>3.4299999999999997E-2</v>
+      </c>
+      <c r="U11">
+        <v>4.82</v>
+      </c>
+      <c r="V11">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="W11">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>